<commit_message>
lehigh xls update formatting
</commit_message>
<xml_diff>
--- a/Lehigh_loadshapes/Lehigh_energy_modeling.xlsx
+++ b/Lehigh_loadshapes/Lehigh_energy_modeling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt2/Documents/NRECA/MicrogridUp/microgridup/Lehigh_loadshapes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dpinney/gdrive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74753A6D-246E-9E43-BF59-603270821E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF2E4667-3B85-4A4D-A25E-4136FC3C425B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28260" windowHeight="16640" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
   </bookViews>
   <sheets>
     <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId1"/>
@@ -330,12 +330,6 @@
     <t>LoadShape file</t>
   </si>
   <si>
-    <t>$/kWh</t>
-  </si>
-  <si>
-    <t>$/kw/month</t>
-  </si>
-  <si>
     <t>6_building_resid_combined_11032020.csv</t>
   </si>
   <si>
@@ -457,6 +451,12 @@
   </si>
   <si>
     <t>Smallest individual load is not cost effective to island</t>
+  </si>
+  <si>
+    <t>peak demand charge $/kw/month</t>
+  </si>
+  <si>
+    <t>power cost $/kWh</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -493,6 +493,23 @@
       <color rgb="FF333333"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -514,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -527,8 +544,17 @@
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,21 +869,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C66B282-24B3-4444-829E-2D855F3D6C7A}">
-  <dimension ref="A4:N32"/>
+  <dimension ref="A4:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" customWidth="1"/>
-    <col min="9" max="9" width="18.5" customWidth="1"/>
-    <col min="11" max="11" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
     <col min="12" max="12" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -876,7 +903,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="102">
+    <row r="7" spans="1:11" ht="85">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1165,7 +1192,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
@@ -1184,12 +1211,12 @@
         <v>6264</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G17">
         <v>13140000</v>
@@ -1204,338 +1231,369 @@
         <v>2975</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="85">
-      <c r="A22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="85">
+      <c r="A22" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+    </row>
+    <row r="23" spans="1:15" ht="85" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" ht="86">
-      <c r="A23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23">
+      <c r="C23" s="8">
         <v>0.1</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="8">
         <v>20</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="8">
         <f>7*24</f>
         <v>168</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I23" s="5">
+      <c r="G23" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="12">
         <v>1645427</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="9">
         <v>292</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="9">
         <v>77</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="L23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+    </row>
+    <row r="24" spans="1:15" ht="68" customHeight="1">
+      <c r="A24" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D24" s="8">
+        <v>20</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="8">
+        <v>24</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="I24" s="12">
+        <v>2294249</v>
+      </c>
+      <c r="J24" s="8">
+        <v>281</v>
+      </c>
+      <c r="K24" s="8">
+        <v>74</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+    </row>
+    <row r="25" spans="1:15" ht="68" customHeight="1">
+      <c r="A25" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="8">
+        <v>20</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="8">
+        <v>168</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-    </row>
-    <row r="24" spans="1:14" ht="69">
-      <c r="A24" s="2" t="s">
+      <c r="I25" s="13">
+        <v>2180251</v>
+      </c>
+      <c r="J25" s="11">
         <v>117</v>
       </c>
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24">
+      <c r="K25" s="8">
+        <v>27</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+    </row>
+    <row r="26" spans="1:15" ht="68" customHeight="1">
+      <c r="A26" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="8">
         <v>0.1</v>
       </c>
-      <c r="D24">
+      <c r="D26" s="8">
         <v>20</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E26" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F24">
-        <v>24</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="I24" s="5">
-        <v>2294249</v>
-      </c>
-      <c r="J24">
-        <v>281</v>
-      </c>
-      <c r="K24">
-        <v>74</v>
-      </c>
-      <c r="L24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="69">
-      <c r="A25" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25">
-        <v>0.1</v>
-      </c>
-      <c r="D25">
-        <v>20</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25">
-        <v>168</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="I25" s="9">
-        <v>2180251</v>
-      </c>
-      <c r="J25" s="8">
-        <v>117</v>
-      </c>
-      <c r="K25">
-        <v>27</v>
-      </c>
-      <c r="L25" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="68">
-      <c r="A26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26">
-        <v>0.1</v>
-      </c>
-      <c r="D26">
-        <v>20</v>
-      </c>
-      <c r="E26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26">
+      <c r="F26" s="8">
         <f>7*24</f>
         <v>168</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I26" s="9">
+      <c r="G26" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" s="13">
         <v>937421</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="8">
         <v>393</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="8">
         <v>71</v>
       </c>
-      <c r="L26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="69">
-      <c r="A27" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="L26" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+    </row>
+    <row r="27" spans="1:15" ht="68">
+      <c r="A27" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="8">
         <v>0.1</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="8">
         <v>20</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="8">
         <f>7*24</f>
         <v>168</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I27" s="5">
+      <c r="G27" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="10">
         <v>-12437</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="8">
         <v>544</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="8">
         <v>77</v>
       </c>
-      <c r="L27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="69">
-      <c r="A28" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="L27" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+    </row>
+    <row r="28" spans="1:15" ht="68" customHeight="1">
+      <c r="A28" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="8">
+        <v>20</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" ref="F28:F29" si="1">7*24</f>
+        <v>168</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H28" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C28">
+      <c r="I28" s="12">
+        <v>185930</v>
+      </c>
+      <c r="J28" s="8">
+        <v>316</v>
+      </c>
+      <c r="K28" s="8">
+        <v>58</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+    </row>
+    <row r="29" spans="1:15" ht="68">
+      <c r="A29" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="8">
         <v>0.1</v>
       </c>
-      <c r="D28">
+      <c r="D29" s="8">
         <v>20</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F28">
-        <f t="shared" ref="E28:F32" si="1">7*24</f>
-        <v>168</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="I28" s="5">
-        <v>185930</v>
-      </c>
-      <c r="J28">
-        <v>316</v>
-      </c>
-      <c r="K28">
-        <v>58</v>
-      </c>
-      <c r="L28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="69">
-      <c r="A29" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29">
-        <v>0.1</v>
-      </c>
-      <c r="D29">
-        <v>20</v>
-      </c>
-      <c r="E29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29">
+      <c r="F29" s="8">
         <f t="shared" si="1"/>
         <v>168</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I29" s="5">
+      <c r="G29" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" s="10">
         <v>-25266</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="8">
         <v>283</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="8">
         <v>50</v>
       </c>
-      <c r="L29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="L29" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+    </row>
+    <row r="30" spans="1:15">
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:15">
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:15">
       <c r="F32" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="L23:O23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2018,7 +2076,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="2" customFormat="1" ht="68">
+    <row r="35" spans="1:11" s="2" customFormat="1" ht="51">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
updated energy modeling overview
</commit_message>
<xml_diff>
--- a/Lehigh_loadshapes/Lehigh_energy_modeling.xlsx
+++ b/Lehigh_loadshapes/Lehigh_energy_modeling.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt2/Documents/NRECA/MicrogridUp/microgridup/Lehigh_loadshapes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5CA1B3-00CB-D54C-814E-633353DC9C36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6292E39C-583A-3F45-AC6B-07F7B3A1C83F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12440" yWindow="-20240" windowWidth="19240" windowHeight="18340" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
+    <workbookView xWindow="18700" yWindow="460" windowWidth="10000" windowHeight="16120" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
   </bookViews>
   <sheets>
-    <sheet name="112020_Lehigh.dss" sheetId="3" r:id="rId1"/>
+    <sheet name="112320_Lehigh.dss" sheetId="3" r:id="rId1"/>
     <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId2"/>
     <sheet name="6_buildings_10282020" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="188">
   <si>
     <t>35 units</t>
   </si>
@@ -469,9 +469,6 @@
     <t>Lehigh.dss 4 microgrid system</t>
   </si>
   <si>
-    <t>Microgrid</t>
-  </si>
-  <si>
     <t>Loads in Lehigh.dss</t>
   </si>
   <si>
@@ -493,9 +490,6 @@
     <t>'632633'</t>
   </si>
   <si>
-    <t>400kW_resid.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Miami, FL;  outage; critical load factor 70%; 2017; 30,000 gallons of diesel (not all of which gets burned)</t>
   </si>
   <si>
@@ -536,6 +530,123 @@
   </si>
   <si>
     <t>*Calculated using all loads connected to gen bus added together</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery_mult_2017.csv was based on the output of a 31.3 kWH, 11.9 kW battery system putting out about 6440 kWH per year in Texas in 2017. The loadshape is scaled to reflect this total production, producing up to 100% of total kW output in one hour.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">solar_mult_2017.csv was based on the REopt financial analysis output (with no specified outages!) of a 400 kW pv system putting out on average 650,000 kWH per year in Texas in 2017. The loadshape is scaled to reflect this total production, producing up to 75% of total kVA of the solar panels at one time.  </t>
+  </si>
+  <si>
+    <t>Solar_mult_2017, battery_mult_2017 and diesel_mult_2017 work together within the same microgrid to balance eachother's load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diesel_mult_2017.csv was based on the output of a 107 kVA diesel generato in Texas in 2017. The loadshape is scaled to reflect high utility rate production using diesel to shave peak demand during the summer months mostly, producing up to 100% of total kW output in one hour.  </t>
+  </si>
+  <si>
+    <t>Json converter: https://onlinejsontools.com/convert-json-to-text</t>
+  </si>
+  <si>
+    <t>Reopt API docs: https://developer.nrel.gov/docs/energy-optimization/reopt-v1/</t>
+  </si>
+  <si>
+    <t>634a</t>
+  </si>
+  <si>
+    <t>634b</t>
+  </si>
+  <si>
+    <t>634c</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>'675a','675b','675c'</t>
+  </si>
+  <si>
+    <t>675a</t>
+  </si>
+  <si>
+    <t>675b</t>
+  </si>
+  <si>
+    <t>675c</t>
+  </si>
+  <si>
+    <t>671692'</t>
+  </si>
+  <si>
+    <t>'675'</t>
+  </si>
+  <si>
+    <t>400kW_resid.txt</t>
+  </si>
+  <si>
+    <t>'611','652'</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>'671684'</t>
+  </si>
+  <si>
+    <t>m4</t>
+  </si>
+  <si>
+    <t>'645','646'</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>hospital.txt</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>medium_office.txt</t>
+  </si>
+  <si>
+    <t>Hangar</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>Operations Center</t>
+  </si>
+  <si>
+    <t>supermarket.txt</t>
+  </si>
+  <si>
+    <t>hotel_medium.tx</t>
+  </si>
+  <si>
+    <t>warehouse.txt</t>
+  </si>
+  <si>
+    <t>Data Center</t>
+  </si>
+  <si>
+    <t>*To build the demand_loads for each microgrid, I used the associated csv column, adjusted to the max load, and added the shapes together, loading it into the save "1606" run from Reopt web tool on 11/19/2020</t>
+  </si>
+  <si>
+    <t>m2_load.csv</t>
+  </si>
+  <si>
+    <t>m3_load.csv</t>
+  </si>
+  <si>
+    <t>m4_load.csv</t>
+  </si>
+  <si>
+    <t>*I am not sure that the NPV includes capital cost?</t>
+  </si>
+  <si>
+    <t>*minimum survived outage is often 0 hours</t>
   </si>
 </sst>
 </file>
@@ -545,7 +656,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -572,6 +683,12 @@
       <color rgb="FF333333"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -593,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -608,6 +725,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446EF4BD-D0A2-FC45-BEE7-33012DE4E129}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -937,7 +1055,7 @@
     <col min="6" max="6" width="22.5" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="10" max="11" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="22.5" customWidth="1"/>
     <col min="13" max="13" width="18.83203125" customWidth="1"/>
@@ -950,57 +1068,91 @@
         <v>127</v>
       </c>
     </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>154</v>
+      </c>
+    </row>
     <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:23">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
       <c r="O6" t="s">
         <v>45</v>
       </c>
       <c r="P6" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="I8" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8">
+        <f>133/331</f>
+        <v>0.40181268882175225</v>
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="G9" t="s">
-        <v>150</v>
+      <c r="I9" t="s">
+        <v>148</v>
       </c>
       <c r="O9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S9" t="s">
-        <v>144</v>
+        <v>142</v>
+      </c>
+      <c r="T9" t="s">
+        <v>186</v>
+      </c>
+      <c r="U9" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="48" customHeight="1">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" t="s">
         <v>129</v>
       </c>
-      <c r="C10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D10" t="s">
-        <v>130</v>
-      </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F10" t="s">
         <v>88</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J10" t="s">
         <v>89</v>
@@ -1018,19 +1170,19 @@
         <v>71</v>
       </c>
       <c r="O10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="R10" s="2" t="s">
+      <c r="S10" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>107</v>
@@ -1047,31 +1199,28 @@
     </row>
     <row r="11" spans="1:23" ht="17">
       <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
         <v>132</v>
       </c>
-      <c r="B11" t="s">
-        <v>133</v>
-      </c>
       <c r="C11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D11">
         <v>634</v>
       </c>
-      <c r="E11" t="s">
-        <v>145</v>
-      </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="G11">
+        <v>400</v>
+      </c>
+      <c r="H11">
         <v>178.38</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>63.57</v>
-      </c>
-      <c r="I11">
-        <v>400</v>
       </c>
       <c r="J11">
         <v>0.1</v>
@@ -1115,7 +1264,380 @@
         <v>77</v>
       </c>
     </row>
+    <row r="12" spans="1:23">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="17">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G15">
+        <v>772.9</v>
+      </c>
+      <c r="H15">
+        <v>426</v>
+      </c>
+      <c r="I15">
+        <v>217</v>
+      </c>
+      <c r="J15">
+        <v>0.1</v>
+      </c>
+      <c r="K15">
+        <v>20</v>
+      </c>
+      <c r="L15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O15">
+        <v>265</v>
+      </c>
+      <c r="P15">
+        <v>1234</v>
+      </c>
+      <c r="Q15">
+        <v>198</v>
+      </c>
+      <c r="R15">
+        <v>553</v>
+      </c>
+      <c r="S15">
+        <f>O15*500+P15*1600+R15*420+Q15*840</f>
+        <v>2505480</v>
+      </c>
+      <c r="T15">
+        <v>214920</v>
+      </c>
+      <c r="U15">
+        <v>307</v>
+      </c>
+      <c r="V15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" t="s">
+        <v>172</v>
+      </c>
+      <c r="G16">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G17">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="17">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19">
+        <v>684</v>
+      </c>
+      <c r="F19" t="s">
+        <v>184</v>
+      </c>
+      <c r="G19">
+        <f>170+128</f>
+        <v>298</v>
+      </c>
+      <c r="H19">
+        <v>127.7</v>
+      </c>
+      <c r="I19">
+        <v>53.33</v>
+      </c>
+      <c r="J19">
+        <v>0.1</v>
+      </c>
+      <c r="K19">
+        <v>20</v>
+      </c>
+      <c r="L19" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O19">
+        <v>81</v>
+      </c>
+      <c r="P19">
+        <v>432</v>
+      </c>
+      <c r="Q19">
+        <v>83</v>
+      </c>
+      <c r="R19">
+        <v>225</v>
+      </c>
+      <c r="S19">
+        <f>O19*500+P19*1600+R19*420+Q19*840</f>
+        <v>895920</v>
+      </c>
+      <c r="T19">
+        <v>109888</v>
+      </c>
+      <c r="U19">
+        <v>1067</v>
+      </c>
+      <c r="V19">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20">
+        <v>611</v>
+      </c>
+      <c r="E20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G20">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21">
+        <v>652</v>
+      </c>
+      <c r="E21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="17">
+      <c r="A22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22">
+        <v>632645</v>
+      </c>
+      <c r="D22">
+        <v>646</v>
+      </c>
+      <c r="F22" t="s">
+        <v>185</v>
+      </c>
+      <c r="G22">
+        <v>363</v>
+      </c>
+      <c r="H22">
+        <v>231</v>
+      </c>
+      <c r="I22">
+        <v>89</v>
+      </c>
+      <c r="J22">
+        <v>0.1</v>
+      </c>
+      <c r="K22">
+        <v>20</v>
+      </c>
+      <c r="L22" t="s">
+        <v>50</v>
+      </c>
+      <c r="M22">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O22">
+        <v>145</v>
+      </c>
+      <c r="P22">
+        <v>590</v>
+      </c>
+      <c r="Q22">
+        <v>98</v>
+      </c>
+      <c r="R22">
+        <v>346</v>
+      </c>
+      <c r="S22">
+        <f>O22*500+P22*1600+R22*420+Q22*840</f>
+        <v>1244140</v>
+      </c>
+      <c r="T22">
+        <v>20343</v>
+      </c>
+      <c r="U22">
+        <v>216</v>
+      </c>
+      <c r="V22">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23">
+        <v>645</v>
+      </c>
+      <c r="E23" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" t="s">
+        <v>179</v>
+      </c>
+      <c r="G23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24">
+        <v>646</v>
+      </c>
+      <c r="E24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" t="s">
+        <v>178</v>
+      </c>
+      <c r="G24">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1124,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C66B282-24B3-4444-829E-2D855F3D6C7A}">
   <dimension ref="A4:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>